<commit_message>
feat: last changes in august
</commit_message>
<xml_diff>
--- a/media/pattern/data.xlsx
+++ b/media/pattern/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,7 +775,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1950000.0</t>
+          <t>3150000.0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -802,7 +802,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1237.3333333333333</t>
+          <t>2060.5333333333333</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>540000.0</t>
+          <t>900000.0</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>8686.875</t>
+          <t>9534.375</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -910,7 +910,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7020.0</t>
+          <t>7560.0</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>7800.623999999998</t>
+          <t>8400.671999999999</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3450000.0</t>
+          <t>8050000.0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1550000.0</t>
+          <t>2650000.0</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>704000.0</t>
+          <t>1056000.0</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>840000.0</t>
+          <t>1260000.0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>202472.0</t>
+          <t>303708.0</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>796000.0</t>
+          <t>1194000.0</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1116664.0</t>
+          <t>1674996.0</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1207,7 +1207,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>666664.0</t>
+          <t>999996.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>874000.0</t>
+          <t>1311000.0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>437636.0</t>
+          <t>656454.0</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>740000.0</t>
+          <t>1110000.0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1000000.0</t>
+          <t>1500000.0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>516000.0</t>
+          <t>774000.0</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7843353.0</t>
+          <t>7845967.451</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2739585.0</t>
+          <t>3652780.0</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>3375.0</t>
+          <t>4125.0</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1612,7 +1612,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1024.08</t>
+          <t>1365.44</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1680.0</t>
+          <t>2240.0</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1470.0</t>
+          <t>1960.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1500.4499999999998</t>
+          <t>2000.6</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>630.0</t>
+          <t>3150.0</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>789</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1801,10 +1801,361 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>354</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Блоггеры</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Максима Телеком ( Qvant)wi-fi.ru</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Блоггеры</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Максима Телеком ( Qvant)wi-fi.ru</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Блоггеры</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Максима Телеком ( Qvant)wi-fi.ru</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Smart TVGPMD</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>330.0</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Smart TVGPMD</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>330.0</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Smart TVИМХО</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>845000.0</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Блоггеры</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Максима Телеком ( Qvant)wi-fi.ru</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>300.0</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Пакет XL Flex Rambler&amp;Сo Desktop+Mobile Reach Video PMP</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>1350.0</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Пакет XL Flex Rambler&amp;Сo Desktop+Mobile Reach Video PMP</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>1350.0</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
         <is>
           <t>None</t>
         </is>

</xml_diff>